<commit_message>
small edits to files
</commit_message>
<xml_diff>
--- a/Datasets/Combined datasets/elec_ps.xlsx
+++ b/Datasets/Combined datasets/elec_ps.xlsx
@@ -174,19 +174,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>91.577720642089844</v>
+        <v>22.761026382446289</v>
       </c>
       <c r="C2">
-        <v>88.593040466308594</v>
+        <v>8.3560733795166016</v>
       </c>
       <c r="D2">
-        <v>79.215652465820312</v>
+        <v>42.763835906982422</v>
       </c>
       <c r="E2">
-        <v>108.20364379882812</v>
+        <v>23.33671760559082</v>
       </c>
       <c r="F2">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -194,19 +194,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>106.89147186279297</v>
+        <v>29.816822052001953</v>
       </c>
       <c r="C3">
-        <v>106.10771942138672</v>
+        <v>31.184486389160156</v>
       </c>
       <c r="D3">
-        <v>100.70633697509766</v>
+        <v>14.060967445373535</v>
       </c>
       <c r="E3">
-        <v>114.19622802734375</v>
+        <v>43.618869781494141</v>
       </c>
       <c r="F3">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -214,19 +214,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>104.42478942871094</v>
+        <v>17.641729354858398</v>
       </c>
       <c r="C4">
-        <v>95.14447021484375</v>
+        <v>7.90362548828125</v>
       </c>
       <c r="D4">
-        <v>105.07274627685547</v>
+        <v>35.480567932128906</v>
       </c>
       <c r="E4">
-        <v>117.03443145751953</v>
+        <v>13.714466094970703</v>
       </c>
       <c r="F4">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -234,19 +234,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>122.30293273925781</v>
+        <v>12.664560317993164</v>
       </c>
       <c r="C5">
-        <v>115.0987548828125</v>
+        <v>10.947165489196777</v>
       </c>
       <c r="D5">
-        <v>120.43034362792969</v>
+        <v>17.053176879882812</v>
       </c>
       <c r="E5">
-        <v>134.46719360351562</v>
+        <v>10.729365348815918</v>
       </c>
       <c r="F5">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -254,19 +254,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>78.644371032714844</v>
+        <v>14.035014152526855</v>
       </c>
       <c r="C6">
-        <v>72.006004333496094</v>
+        <v>4.9732275009155273</v>
       </c>
       <c r="D6">
-        <v>82.153076171875</v>
+        <v>6.6776609420776367</v>
       </c>
       <c r="E6">
-        <v>84.619041442871094</v>
+        <v>34.337776184082031</v>
       </c>
       <c r="F6">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -274,19 +274,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>82.38525390625</v>
+        <v>28.888919830322266</v>
       </c>
       <c r="C7">
-        <v>77.412933349609375</v>
+        <v>27.697607040405273</v>
       </c>
       <c r="D7">
-        <v>86.766525268554688</v>
+        <v>10.719847679138184</v>
       </c>
       <c r="E7">
-        <v>85.1072998046875</v>
+        <v>48.759868621826172</v>
       </c>
       <c r="F7">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -294,19 +294,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>74.562385559082031</v>
+        <v>49.569644927978516</v>
       </c>
       <c r="C8">
-        <v>67.163475036621094</v>
+        <v>40.543010711669922</v>
       </c>
       <c r="D8">
-        <v>64.781761169433594</v>
+        <v>67.994216918945312</v>
       </c>
       <c r="E8">
-        <v>94.912879943847656</v>
+        <v>44.040260314941406</v>
       </c>
       <c r="F8">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
@@ -314,19 +314,15 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>64.67236328125</v>
-      </c>
-      <c r="C9">
-        <v>51.462238311767578</v>
-      </c>
-      <c r="D9">
-        <v>70.781707763671875</v>
-      </c>
+        <v>3.936328649520874</v>
+      </c>
+      <c r="C9"/>
+      <c r="D9"/>
       <c r="E9">
-        <v>77.434623718261719</v>
+        <v>13.495984077453613</v>
       </c>
       <c r="F9">
-        <v>24</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -334,16 +330,16 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>129.14375305175781</v>
+        <v>80.445335388183594</v>
       </c>
       <c r="C10">
-        <v>126.35596466064453</v>
+        <v>83.715087890625</v>
       </c>
       <c r="D10">
-        <v>127.19797515869141</v>
+        <v>71.361358642578125</v>
       </c>
       <c r="E10">
-        <v>135.07208251953125</v>
+        <v>84.858245849609375</v>
       </c>
       <c r="F10">
         <v>24</v>
@@ -354,19 +350,17 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>32.487773895263672</v>
-      </c>
-      <c r="C11">
-        <v>20.081682205200195</v>
-      </c>
+        <v>7.6583642959594727</v>
+      </c>
+      <c r="C11"/>
       <c r="D11">
-        <v>43.688575744628906</v>
+        <v>4.8454499244689941</v>
       </c>
       <c r="E11">
-        <v>39.009960174560547</v>
+        <v>21.411798477172852</v>
       </c>
       <c r="F11">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -374,19 +368,19 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>95.714561462402344</v>
+        <v>42.753768920898438</v>
       </c>
       <c r="C12">
-        <v>79.359039306640625</v>
+        <v>30.814075469970703</v>
       </c>
       <c r="D12">
-        <v>100.60768890380859</v>
+        <v>58.436553955078125</v>
       </c>
       <c r="E12">
-        <v>114.18647003173828</v>
+        <v>44.127696990966797</v>
       </c>
       <c r="F12">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13">
@@ -394,16 +388,16 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>126.81296539306641</v>
+        <v>92.138404846191406</v>
       </c>
       <c r="C13">
-        <v>119.02129364013672</v>
+        <v>81.411460876464844</v>
       </c>
       <c r="D13">
-        <v>124.59197998046875</v>
+        <v>88.749244689941406</v>
       </c>
       <c r="E13">
-        <v>140.16493225097656</v>
+        <v>110.85178375244141</v>
       </c>
       <c r="F13">
         <v>24</v>
@@ -414,19 +408,19 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>129.75340270996094</v>
+        <v>36.334754943847656</v>
       </c>
       <c r="C14">
-        <v>126.24696350097656</v>
+        <v>19.992107391357422</v>
       </c>
       <c r="D14">
-        <v>123.20436859130859</v>
+        <v>54.431446075439453</v>
       </c>
       <c r="E14">
-        <v>141.31163024902344</v>
+        <v>41.584705352783203</v>
       </c>
       <c r="F14">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
@@ -434,19 +428,17 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>119.34193420410156</v>
-      </c>
-      <c r="C15">
-        <v>112.32425689697266</v>
-      </c>
+        <v>5.2237510681152344</v>
+      </c>
+      <c r="C15"/>
       <c r="D15">
-        <v>123.92107391357422</v>
+        <v>10.731805801391602</v>
       </c>
       <c r="E15">
-        <v>124.78804016113281</v>
+        <v>7.1781978607177734</v>
       </c>
       <c r="F15">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -454,16 +446,16 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>132.30894470214844</v>
+        <v>79.771583557128906</v>
       </c>
       <c r="C16">
-        <v>128.47477722167969</v>
+        <v>72.468818664550781</v>
       </c>
       <c r="D16">
-        <v>129.648193359375</v>
+        <v>87.21966552734375</v>
       </c>
       <c r="E16">
-        <v>140.44712829589844</v>
+        <v>82.75604248046875</v>
       </c>
       <c r="F16">
         <v>24</v>
@@ -474,19 +466,19 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>60.593048095703125</v>
+        <v>17.696575164794922</v>
       </c>
       <c r="C17">
-        <v>54.279186248779297</v>
+        <v>13.095124244689941</v>
       </c>
       <c r="D17">
-        <v>53.566493988037109</v>
+        <v>23.841091156005859</v>
       </c>
       <c r="E17">
-        <v>76.639404296875</v>
+        <v>18.125560760498047</v>
       </c>
       <c r="F17">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
@@ -494,19 +486,19 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>101.00479888916016</v>
+        <v>48.864082336425781</v>
       </c>
       <c r="C18">
-        <v>100.98069000244141</v>
+        <v>44.248367309570312</v>
       </c>
       <c r="D18">
-        <v>92.499031066894531</v>
+        <v>56.361957550048828</v>
       </c>
       <c r="E18">
-        <v>109.54500579833984</v>
+        <v>47.960079193115234</v>
       </c>
       <c r="F18">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19">
@@ -514,19 +506,19 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>50.229892730712891</v>
+        <v>11.124140739440918</v>
       </c>
       <c r="C19">
-        <v>48.828453063964844</v>
+        <v>3.3301558494567871</v>
       </c>
       <c r="D19">
-        <v>50.348209381103516</v>
+        <v>20.33515739440918</v>
       </c>
       <c r="E19">
-        <v>52.113620758056641</v>
+        <v>13.047391891479492</v>
       </c>
       <c r="F19">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20">
@@ -534,19 +526,19 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>40.439579010009766</v>
+        <v>11.437325477600098</v>
       </c>
       <c r="C20">
-        <v>37.290592193603516</v>
+        <v>4.9074540138244629</v>
       </c>
       <c r="D20">
-        <v>39.746303558349609</v>
+        <v>10.678426742553711</v>
       </c>
       <c r="E20">
-        <v>45.63140869140625</v>
+        <v>21.524614334106445</v>
       </c>
       <c r="F20">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21">
@@ -554,16 +546,16 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <v>126.35558319091797</v>
+        <v>77.817619323730469</v>
       </c>
       <c r="C21">
-        <v>133.56062316894531</v>
+        <v>81.432975769042969</v>
       </c>
       <c r="D21">
-        <v>106.56439971923828</v>
+        <v>61.681125640869141</v>
       </c>
       <c r="E21">
-        <v>135.85385131835938</v>
+        <v>88.789314270019531</v>
       </c>
       <c r="F21">
         <v>24</v>
@@ -574,19 +566,15 @@
         <v>26</v>
       </c>
       <c r="B22">
-        <v>109.71593475341797</v>
-      </c>
-      <c r="C22">
-        <v>98.229179382324219</v>
-      </c>
+        <v>3.311140775680542</v>
+      </c>
+      <c r="C22"/>
       <c r="D22">
-        <v>102.15428924560547</v>
-      </c>
-      <c r="E22">
-        <v>133.687255859375</v>
-      </c>
+        <v>11.352482795715332</v>
+      </c>
+      <c r="E22"/>
       <c r="F22">
-        <v>24</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -594,19 +582,19 @@
         <v>27</v>
       </c>
       <c r="B23">
-        <v>108.09149932861328</v>
+        <v>26.37989616394043</v>
       </c>
       <c r="C23">
-        <v>101.51231384277344</v>
+        <v>16.366802215576172</v>
       </c>
       <c r="D23">
-        <v>105.14959716796875</v>
+        <v>42.789203643798828</v>
       </c>
       <c r="E23">
-        <v>120.43223571777344</v>
+        <v>24.275009155273438</v>
       </c>
       <c r="F23">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24">
@@ -614,19 +602,19 @@
         <v>28</v>
       </c>
       <c r="B24">
-        <v>121.20050048828125</v>
+        <v>28.481294631958008</v>
       </c>
       <c r="C24">
-        <v>114.33344268798828</v>
+        <v>18.266279220581055</v>
       </c>
       <c r="D24">
-        <v>115.25188446044922</v>
+        <v>47.511791229248047</v>
       </c>
       <c r="E24">
-        <v>136.95918273925781</v>
+        <v>24.043674468994141</v>
       </c>
       <c r="F24">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25">
@@ -634,19 +622,19 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>86.625877380371094</v>
+        <v>58.673992156982422</v>
       </c>
       <c r="C25">
-        <v>82.764823913574219</v>
+        <v>32.936069488525391</v>
       </c>
       <c r="D25">
-        <v>78.539306640625</v>
+        <v>84.05450439453125</v>
       </c>
       <c r="E25">
-        <v>100.22823333740234</v>
+        <v>70.061943054199219</v>
       </c>
       <c r="F25">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>